<commit_message>
Mapa i Klienci PSZOK
</commit_message>
<xml_diff>
--- a/Klienci PSZOK-no-duplicates.xlsx
+++ b/Klienci PSZOK-no-duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7ED3395B-E36C-4DFB-9D15-3EACDB839F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{825EF4D4-6151-4D63-ADA7-17C211712706}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7ED3395B-E36C-4DFB-9D15-3EACDB839F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E465E29D-2F0E-4800-84F7-2432C0746563}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Związek Międzygminny „Gospodarka Komunalna” - Chrzanów</t>
   </si>
@@ -203,10 +203,10 @@
     <t>Gmina Pietrowice Wielkie</t>
   </si>
   <si>
-    <t>Przedsiębiorstwo Usług Komunalnych Kaliska Sp. z o.o. w organizacji</t>
-  </si>
-  <si>
-    <t>Gordon &amp; Great Consulting Sp. z o.o. Sp. k.</t>
+    <t>Przedsiębiorstwo Usług Komunalnych Kaliska Sp. z o.o.</t>
+  </si>
+  <si>
+    <t>Gordon &amp; Great Consulting Sp. z o.o. Sp. k. || Gmina Wierzchosławice</t>
   </si>
   <si>
     <t>Miasto i Gmina Pilawa</t>
@@ -216,15 +216,6 @@
   </si>
   <si>
     <t>Gmina Chojna</t>
-  </si>
-  <si>
-    <t>Przedsiębiorstwo Usług Komunalnych Kaliska Sp. z o.o.</t>
-  </si>
-  <si>
-    <t>Gmina Wierzchosławice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gmina Nisko </t>
   </si>
 </sst>
 </file>
@@ -316,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,7 +332,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -622,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A148"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,19 +924,10 @@
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="A62" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>